<commit_message>
progress on level 1
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="21900" windowHeight="12660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="21900" windowHeight="12660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Hex Edits" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="339">
   <si>
     <t>Value</t>
   </si>
@@ -609,9 +609,6 @@
     <t>(?)</t>
   </si>
   <si>
-    <t>To help you out, I've put outlines around invisible blocks. P-switch activated blocks and doors are still invisible though.</t>
-  </si>
-  <si>
     <t>So Long, Mom…</t>
   </si>
   <si>
@@ -1027,6 +1024,18 @@
   </si>
   <si>
     <t>Fixes garbage that sometimes appears when you touch a spike/Muncher/etc while swimming.</t>
+  </si>
+  <si>
+    <t>_DEVIOUS DINOSAUR_Roses are red, Spinach is green, You turned      into      You killed Yoshi!? You're so mean…</t>
+  </si>
+  <si>
+    <t>Each level except the last has a 3-up moon hidden somewhere. Can you find them all?</t>
+  </si>
+  <si>
+    <t>(second level)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Levels that have a key symbol beside their name have a secret exit. You'll have to work extra hard to find them!  </t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1138,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1167,6 +1176,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1562,7 +1574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1588,7 +1600,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>24</v>
@@ -1608,7 +1620,7 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1625,7 +1637,7 @@
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1642,63 +1654,63 @@
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.25" customHeight="1">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17.25" customHeight="1">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
       <c r="C6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" t="s">
         <v>211</v>
       </c>
-      <c r="D6" t="s">
-        <v>212</v>
-      </c>
       <c r="E6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7" t="s">
+        <v>291</v>
+      </c>
+      <c r="D7" t="s">
         <v>292</v>
       </c>
-      <c r="D7" t="s">
-        <v>293</v>
-      </c>
       <c r="E7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -1707,10 +1719,10 @@
         <v>174</v>
       </c>
       <c r="D8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1786,7 +1798,7 @@
         <v>37</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1800,7 +1812,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1808,13 +1820,13 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1825,7 +1837,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1839,7 +1851,7 @@
         <v>42</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1853,49 +1865,49 @@
         <v>38</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B8" t="s">
         <v>321</v>
-      </c>
-      <c r="B8" t="s">
-        <v>322</v>
       </c>
       <c r="C8" t="s">
         <v>39</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B9" t="s">
         <v>332</v>
-      </c>
-      <c r="B9" t="s">
-        <v>333</v>
       </c>
       <c r="C9" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B10" t="s">
+        <v>302</v>
+      </c>
+      <c r="C10" t="s">
         <v>303</v>
       </c>
-      <c r="C10" t="s">
-        <v>304</v>
-      </c>
       <c r="D10" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1975,12 +1987,12 @@
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -2009,7 +2021,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1">
       <c r="A1" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>57</v>
@@ -2018,7 +2030,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>59</v>
@@ -2035,82 +2047,82 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="C3" t="s">
-        <v>219</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G3" t="s">
         <v>308</v>
-      </c>
-      <c r="F3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G3" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4"/>
       <c r="D4" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E4" t="s">
         <v>316</v>
-      </c>
-      <c r="E4" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5"/>
       <c r="D5" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6"/>
       <c r="D6" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7"/>
       <c r="D7" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8"/>
       <c r="D8" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9"/>
       <c r="D9" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10"/>
       <c r="D10" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2124,30 +2136,30 @@
         <v>72</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E12" t="s">
         <v>63</v>
       </c>
       <c r="F12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="D13" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E13" t="s">
         <v>64</v>
       </c>
       <c r="F13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2167,7 +2179,7 @@
         <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G15" t="s">
         <v>65</v>
@@ -2181,7 +2193,7 @@
         <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2189,7 +2201,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C18" t="s">
         <v>67</v>
@@ -2201,7 +2213,7 @@
         <v>63</v>
       </c>
       <c r="F18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G18" t="s">
         <v>70</v>
@@ -2209,7 +2221,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="B19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>69</v>
@@ -2218,7 +2230,7 @@
         <v>64</v>
       </c>
       <c r="F19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G19" t="s">
         <v>71</v>
@@ -2226,7 +2238,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="B20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2246,10 +2258,10 @@
         <v>63</v>
       </c>
       <c r="F22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2260,7 +2272,7 @@
         <v>66</v>
       </c>
       <c r="F23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2271,18 +2283,18 @@
         <v>66</v>
       </c>
       <c r="F24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="D25" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E25" t="s">
         <v>80</v>
       </c>
       <c r="F25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G25" t="s">
         <v>93</v>
@@ -2290,13 +2302,13 @@
     </row>
     <row r="26" spans="1:7">
       <c r="D26" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E26" t="s">
         <v>91</v>
       </c>
       <c r="F26" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G26" t="s">
         <v>92</v>
@@ -2313,13 +2325,13 @@
         <v>100</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E28" t="s">
         <v>105</v>
       </c>
       <c r="F28" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G28" t="s">
         <v>101</v>
@@ -2340,36 +2352,36 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C32" t="s">
         <v>110</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E32" t="s">
         <v>111</v>
       </c>
       <c r="F32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G32" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="B33" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E33" t="s">
         <v>112</v>
       </c>
       <c r="F33" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G33" t="s">
         <v>113</v>
@@ -2377,7 +2389,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="B34" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G34" t="s">
         <v>114</v>
@@ -2394,13 +2406,13 @@
         <v>120</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E36" t="s">
         <v>78</v>
       </c>
       <c r="F36" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G36" t="s">
         <v>126</v>
@@ -2408,13 +2420,13 @@
     </row>
     <row r="37" spans="1:7">
       <c r="D37" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E37" t="s">
         <v>124</v>
       </c>
       <c r="F37" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G37" t="s">
         <v>127</v>
@@ -2422,13 +2434,13 @@
     </row>
     <row r="38" spans="1:7">
       <c r="D38" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E38" t="s">
         <v>123</v>
       </c>
       <c r="F38" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G38" t="s">
         <v>128</v>
@@ -2436,38 +2448,38 @@
     </row>
     <row r="39" spans="1:7">
       <c r="D39" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E39" t="s">
         <v>121</v>
       </c>
       <c r="F39" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G39" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="D40" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E40" t="s">
         <v>122</v>
       </c>
       <c r="F40" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="D41" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E41" t="s">
         <v>125</v>
       </c>
       <c r="F41" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2481,13 +2493,13 @@
         <v>116</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E43" t="s">
         <v>66</v>
       </c>
       <c r="F43" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G43" t="s">
         <v>117</v>
@@ -2503,19 +2515,19 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C46" t="s">
         <v>107</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E46" t="s">
         <v>66</v>
       </c>
       <c r="F46" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G46" t="s">
         <v>108</v>
@@ -2543,7 +2555,7 @@
         <v>78</v>
       </c>
       <c r="F49" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G49" t="s">
         <v>81</v>
@@ -2557,7 +2569,7 @@
         <v>79</v>
       </c>
       <c r="F50" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G50" t="s">
         <v>82</v>
@@ -2571,7 +2583,7 @@
         <v>80</v>
       </c>
       <c r="F51" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G51" t="s">
         <v>83</v>
@@ -2582,19 +2594,19 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C53" t="s">
         <v>104</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E53" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F53" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G53" t="s">
         <v>169</v>
@@ -2602,13 +2614,13 @@
     </row>
     <row r="54" spans="1:7">
       <c r="D54" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E54" t="s">
         <v>167</v>
       </c>
       <c r="F54" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G54" t="s">
         <v>166</v>
@@ -2616,13 +2628,13 @@
     </row>
     <row r="55" spans="1:7">
       <c r="D55" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E55" t="s">
         <v>168</v>
       </c>
       <c r="F55" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G55" t="s">
         <v>106</v>
@@ -2630,13 +2642,13 @@
     </row>
     <row r="56" spans="1:7">
       <c r="D56" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="E56" t="s">
         <v>239</v>
       </c>
-      <c r="E56" t="s">
-        <v>240</v>
-      </c>
       <c r="F56" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2656,21 +2668,21 @@
         <v>96</v>
       </c>
       <c r="F58" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G58" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="D59" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E59" t="s">
         <v>63</v>
       </c>
       <c r="F59" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G59" t="s">
         <v>98</v>
@@ -2678,13 +2690,13 @@
     </row>
     <row r="60" spans="1:7">
       <c r="D60" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E60" t="s">
         <v>80</v>
       </c>
       <c r="F60" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G60" t="s">
         <v>97</v>
@@ -2695,16 +2707,16 @@
         <v>13</v>
       </c>
       <c r="B62" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C62" t="s">
         <v>158</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F62" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G62" t="s">
         <v>186</v>
@@ -2713,7 +2725,7 @@
     <row r="63" spans="1:7">
       <c r="A63"/>
       <c r="G63" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2727,13 +2739,13 @@
         <v>129</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E65" t="s">
         <v>66</v>
       </c>
       <c r="F65" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G65" t="s">
         <v>130</v>
@@ -2747,7 +2759,7 @@
         <v>133</v>
       </c>
       <c r="F66" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G66" t="s">
         <v>131</v>
@@ -2764,13 +2776,13 @@
         <v>74</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E68" t="s">
         <v>105</v>
       </c>
       <c r="F68" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G68" t="s">
         <v>85</v>
@@ -2778,7 +2790,7 @@
     </row>
     <row r="69" spans="1:7">
       <c r="B69" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G69" t="s">
         <v>84</v>
@@ -2786,10 +2798,10 @@
     </row>
     <row r="70" spans="1:7">
       <c r="B70" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G70" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2802,25 +2814,25 @@
         <v>16</v>
       </c>
       <c r="B73" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C73" t="s">
         <v>159</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E73" t="s">
         <v>66</v>
       </c>
       <c r="F73" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74"/>
       <c r="B74" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2831,36 +2843,36 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C77" t="s">
         <v>66</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E77" t="s">
         <v>66</v>
       </c>
       <c r="F77" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G77" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="B78" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E78" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F78" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2868,22 +2880,22 @@
         <v>18</v>
       </c>
       <c r="B80" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C80" t="s">
         <v>66</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E80" t="s">
         <v>66</v>
       </c>
       <c r="F80" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G80" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2903,7 +2915,7 @@
         <v>66</v>
       </c>
       <c r="F82" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2923,7 +2935,7 @@
         <v>66</v>
       </c>
       <c r="F84" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2943,7 +2955,7 @@
         <v>135</v>
       </c>
       <c r="F86" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2954,7 +2966,7 @@
         <v>136</v>
       </c>
       <c r="F87" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2965,7 +2977,7 @@
         <v>137</v>
       </c>
       <c r="F88" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2976,7 +2988,7 @@
         <v>138</v>
       </c>
       <c r="F89" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2987,7 +2999,7 @@
         <v>125</v>
       </c>
       <c r="F90" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="1:6" s="7" customFormat="1">
@@ -2996,13 +3008,13 @@
     </row>
     <row r="93" spans="1:6" s="14" customFormat="1">
       <c r="A93" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D93" s="15"/>
     </row>
     <row r="94" spans="1:6" s="7" customFormat="1">
       <c r="A94" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>27</v>
@@ -3014,7 +3026,7 @@
         <v>119</v>
       </c>
       <c r="B96" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -3022,7 +3034,7 @@
         <v>92</v>
       </c>
       <c r="B97" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -3033,10 +3045,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3047,7 +3059,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="2" customFormat="1">
@@ -3068,7 +3080,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B4" t="s">
         <v>189</v>
@@ -3079,7 +3091,7 @@
         <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3102,18 +3114,23 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>195</v>
+        <v>337</v>
       </c>
       <c r="B9" t="s">
-        <v>196</v>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3121,7 +3138,7 @@
         <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -3129,12 +3146,12 @@
         <v>162</v>
       </c>
       <c r="B15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="B16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3142,10 +3159,10 @@
         <v>56</v>
       </c>
       <c r="B17" t="s">
+        <v>199</v>
+      </c>
+      <c r="C17" t="s">
         <v>200</v>
-      </c>
-      <c r="C17" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3153,114 +3170,122 @@
         <v>155</v>
       </c>
       <c r="B19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="B20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" t="s">
-        <v>204</v>
+        <v>156</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>195</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>271</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B25" t="s">
-        <v>206</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>204</v>
       </c>
       <c r="B27" t="s">
-        <v>267</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>271</v>
+      </c>
+      <c r="B31" t="s">
         <v>272</v>
       </c>
-      <c r="B29" t="s">
+    </row>
+    <row r="32" spans="1:3">
+      <c r="B32" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="B30" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="7" customFormat="1"/>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:3" s="7" customFormat="1"/>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="2" customFormat="1">
+      <c r="A37" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1">
-      <c r="A35" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="11">
+    <row r="38" spans="1:3">
+      <c r="A38" s="11">
         <v>1</v>
       </c>
-      <c r="B36" t="s">
-        <v>266</v>
-      </c>
-      <c r="C36" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="11">
+      <c r="B38" t="s">
+        <v>265</v>
+      </c>
+      <c r="C38" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="11">
         <v>2</v>
       </c>
-      <c r="B37" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" s="7" customFormat="1"/>
-    <row r="41" spans="1:3" s="9" customFormat="1">
-      <c r="A41" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="B42" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="B43" t="s">
-        <v>265</v>
+      <c r="B39" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="7" customFormat="1"/>
+    <row r="43" spans="1:3" s="9" customFormat="1">
+      <c r="A43" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="B44" t="s">
-        <v>302</v>
+        <v>263</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="B45" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="B46" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -3381,22 +3406,22 @@
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
level 1 progress; some map16 changes
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="340">
   <si>
     <t>Value</t>
   </si>
@@ -600,15 +600,9 @@
     <t>(first level)</t>
   </si>
   <si>
-    <t>You will always start a level as small Mario with no Yoshi and no reserve item. Double-grabbing has been disabled.</t>
-  </si>
-  <si>
     <t>You may have to use a glitch or an exploit to pass a level. I suggest you make frequent alternate saves.</t>
   </si>
   <si>
-    <t>(?)</t>
-  </si>
-  <si>
     <t>So Long, Mom…</t>
   </si>
   <si>
@@ -633,9 +627,6 @@
     <t>This place looks awfully familiar, doesn't it?</t>
   </si>
   <si>
-    <t>Rope Things</t>
-  </si>
-  <si>
     <t>You can probably get to that rope right there, if you really try hard enough …</t>
   </si>
   <si>
@@ -831,9 +822,6 @@
     <t>Welcome to Friendly Mario World (Puzzle Edition) Here you will find levels that test both your puzzle solving and…</t>
   </si>
   <si>
-    <t>Levels that have a key symbol beside their name have a secret exit. You'll have to work extra hard to find them!</t>
-  </si>
-  <si>
     <t>Wings Wings Wings</t>
   </si>
   <si>
@@ -1036,6 +1024,21 @@
   </si>
   <si>
     <t xml:space="preserve">Levels that have a key symbol beside their name have a secret exit. You'll have to work extra hard to find them!  </t>
+  </si>
+  <si>
+    <t>Fixes wall-jump and note block clipping glitch</t>
+  </si>
+  <si>
+    <t>Walljump/Note Block Glitch Fix</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>Rope plus switch palace corners</t>
+  </si>
+  <si>
+    <t>You will always start a level as small Mario with no Yoshi and no reserve item. Double-grabbing and wall-jumping are both disabled.</t>
   </si>
 </sst>
 </file>
@@ -1572,15 +1575,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="89.42578125" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
@@ -1600,7 +1603,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>24</v>
@@ -1620,7 +1623,7 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1637,7 +1640,7 @@
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1654,63 +1657,63 @@
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.25" customHeight="1">
       <c r="A5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17.25" customHeight="1">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D7" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -1719,37 +1722,54 @@
         <v>174</v>
       </c>
       <c r="D8" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>336</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
+        <v>287</v>
+      </c>
+      <c r="D9" t="s">
+        <v>335</v>
+      </c>
+      <c r="E9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
         <v>178</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A10" t="s">
+    <row r="13" spans="1:6" ht="17.25" customHeight="1">
+      <c r="A13" t="s">
         <v>180</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
         <v>181</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D13" t="s">
         <v>182</v>
       </c>
     </row>
@@ -1760,10 +1780,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1798,7 +1818,7 @@
         <v>37</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1812,7 +1832,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1820,13 +1840,13 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1837,7 +1857,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1851,7 +1871,7 @@
         <v>42</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1865,68 +1885,69 @@
         <v>38</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B8" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C8" t="s">
         <v>39</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B9" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C9" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
-        <v>304</v>
+        <v>337</v>
       </c>
       <c r="B10" t="s">
-        <v>302</v>
+        <v>338</v>
       </c>
       <c r="C10" t="s">
-        <v>303</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>323</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
-        <v>32</v>
+        <v>300</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>25</v>
+        <v>298</v>
+      </c>
+      <c r="C11" t="s">
+        <v>299</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>25</v>
@@ -1934,10 +1955,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>25</v>
@@ -1945,24 +1966,21 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E14" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>25</v>
@@ -1973,10 +1991,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>25</v>
@@ -1985,14 +2003,28 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="4" t="s">
-        <v>268</v>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2021,7 +2053,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1">
       <c r="A1" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>57</v>
@@ -2030,7 +2062,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>59</v>
@@ -2047,82 +2079,82 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4"/>
       <c r="D4" s="4" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E4" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5"/>
       <c r="D5" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="E5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6"/>
       <c r="D6" s="4" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E6" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7"/>
       <c r="D7" s="4" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E7" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8"/>
       <c r="D8" s="4" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E8" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9"/>
       <c r="D9" s="4" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E9" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10"/>
       <c r="D10" s="4" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="E10" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2136,30 +2168,30 @@
         <v>72</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E12" t="s">
         <v>63</v>
       </c>
       <c r="F12" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G12" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="D13" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E13" t="s">
         <v>64</v>
       </c>
       <c r="F13" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G13" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2179,7 +2211,7 @@
         <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G15" t="s">
         <v>65</v>
@@ -2193,7 +2225,7 @@
         <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2201,7 +2233,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C18" t="s">
         <v>67</v>
@@ -2213,7 +2245,7 @@
         <v>63</v>
       </c>
       <c r="F18" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G18" t="s">
         <v>70</v>
@@ -2221,7 +2253,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="B19" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>69</v>
@@ -2230,7 +2262,7 @@
         <v>64</v>
       </c>
       <c r="F19" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G19" t="s">
         <v>71</v>
@@ -2238,7 +2270,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="B20" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2258,10 +2290,10 @@
         <v>63</v>
       </c>
       <c r="F22" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G22" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2272,7 +2304,7 @@
         <v>66</v>
       </c>
       <c r="F23" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -2283,18 +2315,18 @@
         <v>66</v>
       </c>
       <c r="F24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="D25" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E25" t="s">
         <v>80</v>
       </c>
       <c r="F25" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G25" t="s">
         <v>93</v>
@@ -2302,13 +2334,13 @@
     </row>
     <row r="26" spans="1:7">
       <c r="D26" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E26" t="s">
         <v>91</v>
       </c>
       <c r="F26" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G26" t="s">
         <v>92</v>
@@ -2325,13 +2357,13 @@
         <v>100</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E28" t="s">
         <v>105</v>
       </c>
       <c r="F28" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G28" t="s">
         <v>101</v>
@@ -2352,36 +2384,36 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C32" t="s">
         <v>110</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E32" t="s">
         <v>111</v>
       </c>
       <c r="F32" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G32" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="B33" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E33" t="s">
         <v>112</v>
       </c>
       <c r="F33" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G33" t="s">
         <v>113</v>
@@ -2389,7 +2421,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="B34" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="G34" t="s">
         <v>114</v>
@@ -2406,13 +2438,13 @@
         <v>120</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E36" t="s">
         <v>78</v>
       </c>
       <c r="F36" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G36" t="s">
         <v>126</v>
@@ -2420,13 +2452,13 @@
     </row>
     <row r="37" spans="1:7">
       <c r="D37" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E37" t="s">
         <v>124</v>
       </c>
       <c r="F37" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G37" t="s">
         <v>127</v>
@@ -2434,13 +2466,13 @@
     </row>
     <row r="38" spans="1:7">
       <c r="D38" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E38" t="s">
         <v>123</v>
       </c>
       <c r="F38" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G38" t="s">
         <v>128</v>
@@ -2448,38 +2480,38 @@
     </row>
     <row r="39" spans="1:7">
       <c r="D39" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E39" t="s">
         <v>121</v>
       </c>
       <c r="F39" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G39" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="D40" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E40" t="s">
         <v>122</v>
       </c>
       <c r="F40" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="D41" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E41" t="s">
         <v>125</v>
       </c>
       <c r="F41" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2493,13 +2525,13 @@
         <v>116</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E43" t="s">
         <v>66</v>
       </c>
       <c r="F43" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G43" t="s">
         <v>117</v>
@@ -2515,19 +2547,19 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C46" t="s">
         <v>107</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E46" t="s">
         <v>66</v>
       </c>
       <c r="F46" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G46" t="s">
         <v>108</v>
@@ -2555,7 +2587,7 @@
         <v>78</v>
       </c>
       <c r="F49" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G49" t="s">
         <v>81</v>
@@ -2569,7 +2601,7 @@
         <v>79</v>
       </c>
       <c r="F50" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G50" t="s">
         <v>82</v>
@@ -2583,7 +2615,7 @@
         <v>80</v>
       </c>
       <c r="F51" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G51" t="s">
         <v>83</v>
@@ -2594,19 +2626,19 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C53" t="s">
         <v>104</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E53" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F53" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G53" t="s">
         <v>169</v>
@@ -2614,13 +2646,13 @@
     </row>
     <row r="54" spans="1:7">
       <c r="D54" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E54" t="s">
         <v>167</v>
       </c>
       <c r="F54" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G54" t="s">
         <v>166</v>
@@ -2628,13 +2660,13 @@
     </row>
     <row r="55" spans="1:7">
       <c r="D55" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E55" t="s">
         <v>168</v>
       </c>
       <c r="F55" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G55" t="s">
         <v>106</v>
@@ -2642,13 +2674,13 @@
     </row>
     <row r="56" spans="1:7">
       <c r="D56" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E56" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F56" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2668,21 +2700,21 @@
         <v>96</v>
       </c>
       <c r="F58" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G58" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="D59" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E59" t="s">
         <v>63</v>
       </c>
       <c r="F59" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G59" t="s">
         <v>98</v>
@@ -2690,13 +2722,13 @@
     </row>
     <row r="60" spans="1:7">
       <c r="D60" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E60" t="s">
         <v>80</v>
       </c>
       <c r="F60" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G60" t="s">
         <v>97</v>
@@ -2707,16 +2739,16 @@
         <v>13</v>
       </c>
       <c r="B62" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C62" t="s">
         <v>158</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F62" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G62" t="s">
         <v>186</v>
@@ -2725,7 +2757,7 @@
     <row r="63" spans="1:7">
       <c r="A63"/>
       <c r="G63" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2739,13 +2771,13 @@
         <v>129</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E65" t="s">
         <v>66</v>
       </c>
       <c r="F65" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G65" t="s">
         <v>130</v>
@@ -2759,7 +2791,7 @@
         <v>133</v>
       </c>
       <c r="F66" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G66" t="s">
         <v>131</v>
@@ -2776,13 +2808,13 @@
         <v>74</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E68" t="s">
         <v>105</v>
       </c>
       <c r="F68" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G68" t="s">
         <v>85</v>
@@ -2790,7 +2822,7 @@
     </row>
     <row r="69" spans="1:7">
       <c r="B69" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="G69" t="s">
         <v>84</v>
@@ -2798,10 +2830,10 @@
     </row>
     <row r="70" spans="1:7">
       <c r="B70" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G70" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2814,25 +2846,25 @@
         <v>16</v>
       </c>
       <c r="B73" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C73" t="s">
         <v>159</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E73" t="s">
         <v>66</v>
       </c>
       <c r="F73" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74"/>
       <c r="B74" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2843,36 +2875,36 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C77" t="s">
         <v>66</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E77" t="s">
         <v>66</v>
       </c>
       <c r="F77" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G77" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="B78" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E78" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F78" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2880,22 +2912,22 @@
         <v>18</v>
       </c>
       <c r="B80" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C80" t="s">
         <v>66</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E80" t="s">
         <v>66</v>
       </c>
       <c r="F80" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G80" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2915,7 +2947,7 @@
         <v>66</v>
       </c>
       <c r="F82" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2935,7 +2967,7 @@
         <v>66</v>
       </c>
       <c r="F84" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2955,7 +2987,7 @@
         <v>135</v>
       </c>
       <c r="F86" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2966,7 +2998,7 @@
         <v>136</v>
       </c>
       <c r="F87" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2977,7 +3009,7 @@
         <v>137</v>
       </c>
       <c r="F88" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2988,7 +3020,7 @@
         <v>138</v>
       </c>
       <c r="F89" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2999,7 +3031,7 @@
         <v>125</v>
       </c>
       <c r="F90" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="92" spans="1:6" s="7" customFormat="1">
@@ -3008,13 +3040,13 @@
     </row>
     <row r="93" spans="1:6" s="14" customFormat="1">
       <c r="A93" s="13" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D93" s="15"/>
     </row>
     <row r="94" spans="1:6" s="7" customFormat="1">
       <c r="A94" s="10" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>27</v>
@@ -3026,7 +3058,7 @@
         <v>119</v>
       </c>
       <c r="B96" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -3034,7 +3066,7 @@
         <v>92</v>
       </c>
       <c r="B97" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -3045,10 +3077,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A25" sqref="A24:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3059,7 +3091,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="2" customFormat="1">
@@ -3080,7 +3112,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B4" t="s">
         <v>189</v>
@@ -3091,7 +3123,7 @@
         <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3104,33 +3136,33 @@
         <v>192</v>
       </c>
       <c r="B7" t="s">
-        <v>193</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B9" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B11" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3138,7 +3170,7 @@
         <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -3146,12 +3178,12 @@
         <v>162</v>
       </c>
       <c r="B15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="B16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3159,10 +3191,10 @@
         <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C17" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3170,12 +3202,12 @@
         <v>155</v>
       </c>
       <c r="B19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="B20" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -3183,7 +3215,7 @@
         <v>156</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -3191,101 +3223,93 @@
         <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>195</v>
+        <v>278</v>
       </c>
       <c r="B25" t="s">
-        <v>270</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>204</v>
+        <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>205</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>267</v>
       </c>
       <c r="B29" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>271</v>
-      </c>
-      <c r="B31" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="B32" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="7" customFormat="1"/>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="7" customFormat="1"/>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="2" customFormat="1">
+      <c r="A35" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" s="2" customFormat="1">
-      <c r="A37" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="11">
+      <c r="A36" s="11">
         <v>1</v>
       </c>
-      <c r="B38" t="s">
-        <v>265</v>
-      </c>
-      <c r="C38" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="11">
+      <c r="B36" t="s">
+        <v>262</v>
+      </c>
+      <c r="C36" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="11">
         <v>2</v>
       </c>
-      <c r="B39" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="7" customFormat="1"/>
-    <row r="43" spans="1:3" s="9" customFormat="1">
-      <c r="A43" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>256</v>
+      <c r="B37" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="7" customFormat="1"/>
+    <row r="41" spans="1:3" s="9" customFormat="1">
+      <c r="A41" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="B42" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="B43" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="B44" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="B45" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="B46" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -3406,22 +3430,22 @@
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed sideways muncher exanimation; progress on level 1
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="21900" windowHeight="12660" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="21900" windowHeight="12660"/>
   </bookViews>
   <sheets>
     <sheet name="Hex Edits" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>Fix overworld glitch where music stops playing after a boss battle</t>
   </si>
   <si>
-    <t>Allow direction coins to be used again if yo leave the level and return</t>
-  </si>
-  <si>
     <t>Patch</t>
   </si>
   <si>
@@ -1039,6 +1036,9 @@
   </si>
   <si>
     <t>You will always start a level as small Mario with no Yoshi and no reserve item. Double-grabbing and wall-jumping are both disabled.</t>
+  </si>
+  <si>
+    <t>Allow direction coins to be used again if you leave the level and return</t>
   </si>
 </sst>
 </file>
@@ -1481,13 +1481,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="4"/>
+    <col min="1" max="2" width="9.140625" style="4"/>
+    <col min="3" max="3" width="70.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
@@ -1503,13 +1504,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1553,7 +1554,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>14</v>
+        <v>339</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1591,186 +1592,186 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
       <c r="E2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>175</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
       <c r="E3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
       <c r="E4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.25" customHeight="1">
       <c r="A5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5" t="s">
         <v>205</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D5" t="s">
-        <v>206</v>
-      </c>
       <c r="E5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17.25" customHeight="1">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" t="s">
         <v>207</v>
       </c>
-      <c r="D6" t="s">
-        <v>208</v>
-      </c>
       <c r="E6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>285</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>286</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>287</v>
       </c>
-      <c r="D7" t="s">
-        <v>288</v>
-      </c>
       <c r="E7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>328</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D8" t="s">
         <v>329</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>174</v>
-      </c>
-      <c r="D8" t="s">
-        <v>330</v>
-      </c>
       <c r="E8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
+        <v>177</v>
+      </c>
+      <c r="D11" t="s">
         <v>178</v>
-      </c>
-      <c r="D11" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25" customHeight="1">
       <c r="A13" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
         <v>180</v>
       </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>181</v>
-      </c>
-      <c r="D13" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1795,16 +1796,16 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1812,13 +1813,13 @@
         <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1826,205 +1827,205 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>318</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
         <v>41</v>
       </c>
-      <c r="C6" t="s">
-        <v>42</v>
-      </c>
       <c r="D6" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B8" t="s">
         <v>316</v>
       </c>
-      <c r="B8" t="s">
-        <v>317</v>
-      </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B9" t="s">
         <v>327</v>
       </c>
-      <c r="B9" t="s">
-        <v>328</v>
-      </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B10" t="s">
         <v>337</v>
       </c>
-      <c r="B10" t="s">
-        <v>338</v>
-      </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B11" t="s">
+        <v>297</v>
+      </c>
+      <c r="C11" t="s">
         <v>298</v>
       </c>
-      <c r="C11" t="s">
-        <v>299</v>
-      </c>
       <c r="D11" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
         <v>53</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -2053,25 +2054,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1">
       <c r="A1" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>255</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2079,82 +2080,82 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="C3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G3" t="s">
         <v>303</v>
-      </c>
-      <c r="F3" t="s">
-        <v>249</v>
-      </c>
-      <c r="G3" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4"/>
       <c r="D4" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E4" t="s">
         <v>311</v>
-      </c>
-      <c r="E4" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5"/>
       <c r="D5" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6"/>
       <c r="D6" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7"/>
       <c r="D7" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8"/>
       <c r="D8" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9"/>
       <c r="D9" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10"/>
       <c r="D10" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2162,36 +2163,36 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="D13" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2199,33 +2200,33 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="D16" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2233,44 +2234,44 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="B19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -2278,72 +2279,72 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" t="s">
         <v>86</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="D23" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="D24" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="D25" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="D26" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E26" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26" t="s">
+        <v>245</v>
+      </c>
+      <c r="G26" t="s">
         <v>91</v>
-      </c>
-      <c r="F26" t="s">
-        <v>246</v>
-      </c>
-      <c r="G26" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2351,32 +2352,32 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" t="s">
         <v>99</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28" t="s">
+        <v>245</v>
+      </c>
+      <c r="G28" t="s">
         <v>100</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="E28" t="s">
-        <v>105</v>
-      </c>
-      <c r="F28" t="s">
-        <v>246</v>
-      </c>
-      <c r="G28" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="G29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="G30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -2384,47 +2385,47 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C32" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E32" t="s">
         <v>110</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="E32" t="s">
-        <v>111</v>
-      </c>
       <c r="F32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G32" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="B33" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E33" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" t="s">
+        <v>245</v>
+      </c>
+      <c r="G33" t="s">
         <v>112</v>
-      </c>
-      <c r="F33" t="s">
-        <v>246</v>
-      </c>
-      <c r="G33" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="B34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -2432,86 +2433,86 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="D37" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E37" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F37" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="D38" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F38" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="D39" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F39" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G39" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="D40" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E40" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F40" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="D41" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F41" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2519,27 +2520,27 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" t="s">
         <v>115</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E43" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43" t="s">
+        <v>247</v>
+      </c>
+      <c r="G43" t="s">
         <v>116</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="E43" t="s">
-        <v>66</v>
-      </c>
-      <c r="F43" t="s">
-        <v>248</v>
-      </c>
-      <c r="G43" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="G44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -2547,27 +2548,27 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C46" t="s">
+        <v>106</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E46" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" t="s">
+        <v>247</v>
+      </c>
+      <c r="G46" t="s">
         <v>107</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="E46" t="s">
-        <v>66</v>
-      </c>
-      <c r="F46" t="s">
-        <v>248</v>
-      </c>
-      <c r="G46" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="G47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -2575,50 +2576,50 @@
         <v>10</v>
       </c>
       <c r="B49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" t="s">
         <v>73</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="E49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F49" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="D50" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F50" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="D51" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F51" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2626,61 +2627,61 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E53" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F53" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="D54" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E54" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F54" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G54" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="D55" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E55" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F55" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="D56" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="E56" t="s">
         <v>235</v>
       </c>
-      <c r="E56" t="s">
-        <v>236</v>
-      </c>
       <c r="F56" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2688,50 +2689,50 @@
         <v>12</v>
       </c>
       <c r="B58" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" t="s">
         <v>94</v>
-      </c>
-      <c r="C58" t="s">
-        <v>95</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F58" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G58" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="D59" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F59" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G59" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="D60" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F60" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G60" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2739,25 +2740,25 @@
         <v>13</v>
       </c>
       <c r="B62" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F62" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G62" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63"/>
       <c r="G63" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2765,36 +2766,36 @@
         <v>14</v>
       </c>
       <c r="B65" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C65" t="s">
+        <v>128</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E65" t="s">
+        <v>65</v>
+      </c>
+      <c r="F65" t="s">
+        <v>246</v>
+      </c>
+      <c r="G65" t="s">
         <v>129</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="E65" t="s">
-        <v>66</v>
-      </c>
-      <c r="F65" t="s">
-        <v>247</v>
-      </c>
-      <c r="G65" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="D66" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E66" t="s">
         <v>132</v>
       </c>
-      <c r="E66" t="s">
-        <v>133</v>
-      </c>
       <c r="F66" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G66" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2802,43 +2803,43 @@
         <v>15</v>
       </c>
       <c r="B68" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F68" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G68" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="B69" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="B70" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G70" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="G71" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2846,25 +2847,25 @@
         <v>16</v>
       </c>
       <c r="B73" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C73" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E73" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F73" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74"/>
       <c r="B74" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2875,36 +2876,36 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C77" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E77" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F77" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G77" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="B78" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F78" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2912,22 +2913,22 @@
         <v>18</v>
       </c>
       <c r="B80" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C80" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E80" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F80" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G80" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2935,19 +2936,19 @@
         <v>19</v>
       </c>
       <c r="B82" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C82" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E82" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F82" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2955,19 +2956,19 @@
         <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C84" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E84" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F84" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2975,63 +2976,63 @@
         <v>21</v>
       </c>
       <c r="B86" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C86" t="s">
+        <v>133</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E86" t="s">
         <v>134</v>
       </c>
-      <c r="D86" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E86" t="s">
-        <v>135</v>
-      </c>
       <c r="F86" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="D87" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E87" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F87" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="D88" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E88" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F88" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="D89" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E89" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F89" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="D90" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E90" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F90" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="92" spans="1:6" s="7" customFormat="1">
@@ -3040,25 +3041,25 @@
     </row>
     <row r="93" spans="1:6" s="14" customFormat="1">
       <c r="A93" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D93" s="15"/>
     </row>
     <row r="94" spans="1:6" s="7" customFormat="1">
       <c r="A94" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D94" s="8"/>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B96" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -3066,7 +3067,7 @@
         <v>92</v>
       </c>
       <c r="B97" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -3079,7 +3080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A24:XFD25"/>
     </sheetView>
   </sheetViews>
@@ -3091,182 +3092,182 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="B16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17" t="s">
         <v>197</v>
-      </c>
-      <c r="C17" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="B20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
+        <v>266</v>
+      </c>
+      <c r="B29" t="s">
         <v>267</v>
-      </c>
-      <c r="B29" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="B30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="7" customFormat="1"/>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="2" customFormat="1">
       <c r="A35" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -3274,10 +3275,10 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C36" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -3285,31 +3286,31 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="7" customFormat="1"/>
     <row r="41" spans="1:3" s="9" customFormat="1">
       <c r="A41" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="B42" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="B43" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="B44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -3330,122 +3331,122 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>